<commit_message>
Atualizar dashboard com novos dados
</commit_message>
<xml_diff>
--- a/public/data/downside_risk_-_month.xlsx
+++ b/public/data/downside_risk_-_month.xlsx
@@ -613,94 +613,94 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>25.41633749944444</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>18.41633749944444</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>-31.08366250055556</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>-12677810.61418092</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>4445455.5358912</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>4977535.535891199</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>115920</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>-648000</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>-8232355.078289717</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>-1934292.577485825</v>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
+        <v>-2609320.836849391</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>-1780789.382606668</v>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>-2483511.036196622</v>
       </c>
       <c r="V2" t="n">
-        <v>0</v>
+        <v>-121532.4986648176</v>
       </c>
       <c r="W2" t="n">
-        <v>0</v>
+        <v>-169361.6747855832</v>
       </c>
       <c r="X2" t="n">
-        <v>0</v>
+        <v>-619899.126125208</v>
       </c>
       <c r="Y2" t="n">
-        <v>0</v>
+        <v>-884431.953659645</v>
       </c>
       <c r="Z2" t="n">
-        <v>0</v>
+        <v>-10166647.65577554</v>
       </c>
       <c r="AA2" t="n">
-        <v>0</v>
+        <v>-10841675.91513911</v>
       </c>
       <c r="AB2" t="n">
-        <v>0</v>
+        <v>0.7060401833876988</v>
       </c>
       <c r="AC2" t="n">
-        <v>0</v>
+        <v>0.2457751023035986</v>
       </c>
       <c r="AD2" t="n">
-        <v>0</v>
+        <v>0.04818471430870252</v>
       </c>
       <c r="AE2" t="n">
-        <v>0</v>
+        <v>0.7020913581522319</v>
       </c>
       <c r="AF2" t="n">
-        <v>0</v>
+        <v>0.2500299062447857</v>
       </c>
       <c r="AG2" t="n">
-        <v>0</v>
+        <v>0.04787873560298232</v>
       </c>
     </row>
     <row r="3">
@@ -716,94 +716,94 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>-11.08456720369892</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>4.050000000000001</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>-15.13456720369892</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>-22.5</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>-30.63456720369892</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>42.05</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>-6449528.570362898</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>-3030475.7998656</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>-2474075.399865601</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>69303.59999999998</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>-625704</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>-9480004.370228494</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>-804362.8389128966</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
+        <v>-1112800.127086782</v>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>-736290.6492241528</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>-1038520.451548273</v>
       </c>
       <c r="V3" t="n">
-        <v>0</v>
+        <v>-4911.552865656839</v>
       </c>
       <c r="W3" t="n">
-        <v>0</v>
+        <v>-6883.539693797571</v>
       </c>
       <c r="X3" t="n">
-        <v>0</v>
+        <v>-322271.4079136542</v>
       </c>
       <c r="Y3" t="n">
-        <v>0</v>
+        <v>-444616.9723478784</v>
       </c>
       <c r="Z3" t="n">
-        <v>0</v>
+        <v>-10284367.20914139</v>
       </c>
       <c r="AA3" t="n">
-        <v>0</v>
+        <v>-10592804.49731527</v>
       </c>
       <c r="AB3" t="n">
-        <v>0</v>
+        <v>0.6923450119479266</v>
       </c>
       <c r="AC3" t="n">
-        <v>0</v>
+        <v>0.303036582085572</v>
       </c>
       <c r="AD3" t="n">
-        <v>0</v>
+        <v>0.004618405966501455</v>
       </c>
       <c r="AE3" t="n">
-        <v>0</v>
+        <v>0.6969837854134193</v>
       </c>
       <c r="AF3" t="n">
-        <v>0</v>
+        <v>0.298396454286556</v>
       </c>
       <c r="AG3" t="n">
-        <v>0</v>
+        <v>0.004619760300024818</v>
       </c>
     </row>
     <row r="4">
@@ -819,94 +819,94 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>-16.23242916711111</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.9100000000000001</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>-17.14242916711111</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>-22.5</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>-32.64242916711111</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>38.91</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>-5752093.083225883</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>-4215061.986100478</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>-3669827.586100478</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>15069.59999999998</v>
       </c>
       <c r="P4" t="n">
-        <v>0</v>
+        <v>-560304</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>-9967155.069326365</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>-1027275.863054189</v>
       </c>
       <c r="S4" t="n">
-        <v>0</v>
+        <v>-1369372.41294406</v>
       </c>
       <c r="T4" t="n">
-        <v>0</v>
+        <v>-996757.0849812323</v>
       </c>
       <c r="U4" t="n">
-        <v>0</v>
+        <v>-1337791.143077626</v>
       </c>
       <c r="V4" t="n">
-        <v>0</v>
+        <v>-813.3308402782592</v>
       </c>
       <c r="W4" t="n">
-        <v>0</v>
+        <v>-1114.464726958156</v>
       </c>
       <c r="X4" t="n">
-        <v>0</v>
+        <v>-239081.2523744593</v>
       </c>
       <c r="Y4" t="n">
-        <v>0</v>
+        <v>-321211.3524074265</v>
       </c>
       <c r="Z4" t="n">
-        <v>0</v>
+        <v>-10994430.93238055</v>
       </c>
       <c r="AA4" t="n">
-        <v>0</v>
+        <v>-11336527.48227043</v>
       </c>
       <c r="AB4" t="n">
-        <v>0</v>
+        <v>0.8060128091164941</v>
       </c>
       <c r="AC4" t="n">
-        <v>0</v>
+        <v>0.1933295029822194</v>
       </c>
       <c r="AD4" t="n">
-        <v>0</v>
+        <v>0.0006576879012865021</v>
       </c>
       <c r="AE4" t="n">
-        <v>0</v>
+        <v>0.805841501014952</v>
       </c>
       <c r="AF4" t="n">
-        <v>0</v>
+        <v>0.1934871819913249</v>
       </c>
       <c r="AG4" t="n">
-        <v>0</v>
+        <v>0.000671316993723038</v>
       </c>
     </row>
     <row r="5">
@@ -922,94 +922,94 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>-25.00186822589247</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>-0.5648400000000002</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>-24.43702822589247</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>-30.5</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>-31.93702822589247</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>37.43516</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>-3877333.793863412</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>-5719285.741817728</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>-5152585.018937729</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>-9665.542079999985</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>-557035.1808</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>-9596619.535681136</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>-1201023.123619514</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>-1605162.979854323</v>
       </c>
       <c r="T5" t="n">
-        <v>0</v>
+        <v>-1196939.197506628</v>
       </c>
       <c r="U5" t="n">
-        <v>0</v>
+        <v>-1584565.849467202</v>
       </c>
       <c r="V5" t="n">
-        <v>0</v>
+        <v>-659.9240747431285</v>
       </c>
       <c r="W5" t="n">
-        <v>0</v>
+        <v>-883.6507079149268</v>
       </c>
       <c r="X5" t="n">
-        <v>0</v>
+        <v>-200184.0307291559</v>
       </c>
       <c r="Y5" t="n">
-        <v>0</v>
+        <v>-266496.6540360064</v>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
+        <v>-10797642.65930065</v>
       </c>
       <c r="AA5" t="n">
-        <v>0</v>
+        <v>-11201782.51553546</v>
       </c>
       <c r="AB5" t="n">
-        <v>0</v>
+        <v>0.8563125085089877</v>
       </c>
       <c r="AC5" t="n">
-        <v>0</v>
+        <v>0.14321536956448</v>
       </c>
       <c r="AD5" t="n">
-        <v>0</v>
+        <v>0.0004721219265322222</v>
       </c>
       <c r="AE5" t="n">
-        <v>0</v>
+        <v>0.8556219876393665</v>
       </c>
       <c r="AF5" t="n">
-        <v>0</v>
+        <v>0.1439008652762511</v>
       </c>
       <c r="AG5" t="n">
-        <v>0</v>
+        <v>0.0004771470843823409</v>
       </c>
     </row>
     <row r="6">
@@ -1025,94 +1025,94 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>-21.45</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>-23.45</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>-63.1</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>9.299999999999997</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>32.35</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>1345235.814203487</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>-5651758.800000001</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>-4005658.800000001</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>40176</v>
       </c>
       <c r="P6" t="n">
-        <v>0</v>
+        <v>-1686276</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>-4306522.985796515</v>
       </c>
       <c r="R6" t="n">
-        <v>0</v>
+        <v>-1053234.860596432</v>
       </c>
       <c r="S6" t="n">
-        <v>0</v>
+        <v>-1374489.93849818</v>
       </c>
       <c r="T6" t="n">
-        <v>0</v>
+        <v>-599166.504562091</v>
       </c>
       <c r="U6" t="n">
-        <v>0</v>
+        <v>-804808.1195427952</v>
       </c>
       <c r="V6" t="n">
-        <v>0</v>
+        <v>-3046.921548767929</v>
       </c>
       <c r="W6" t="n">
-        <v>0</v>
+        <v>-4045.225226504521</v>
       </c>
       <c r="X6" t="n">
-        <v>0</v>
+        <v>-849094.3514765792</v>
       </c>
       <c r="Y6" t="n">
-        <v>0</v>
+        <v>-1148243.673267132</v>
       </c>
       <c r="Z6" t="n">
-        <v>0</v>
+        <v>-5359757.846392947</v>
       </c>
       <c r="AA6" t="n">
-        <v>0</v>
+        <v>-5681012.924294695</v>
       </c>
       <c r="AB6" t="n">
-        <v>0</v>
+        <v>0.4128459268358</v>
       </c>
       <c r="AC6" t="n">
-        <v>0</v>
+        <v>0.5850546414683037</v>
       </c>
       <c r="AD6" t="n">
-        <v>0</v>
+        <v>0.00209943169589633</v>
       </c>
       <c r="AE6" t="n">
-        <v>0</v>
+        <v>0.411225458996542</v>
       </c>
       <c r="AF6" t="n">
-        <v>0</v>
+        <v>0.5867075891920639</v>
       </c>
       <c r="AG6" t="n">
-        <v>0</v>
+        <v>0.002066951811394165</v>
       </c>
     </row>
     <row r="7">
@@ -1128,94 +1128,94 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>-23.24</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>-25.24</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>-63.48</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>8.539999999999999</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>31.7</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>1472891.383151536</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>-5362654.080000001</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>-3919937.280000002</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>36288</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>-1479004.8</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>-3889762.696848463</v>
       </c>
       <c r="R7" t="n">
-        <v>0</v>
+        <v>-966318.0507020823</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>-1252419.119640922</v>
       </c>
       <c r="T7" t="n">
-        <v>0</v>
+        <v>-586344.2782895599</v>
       </c>
       <c r="U7" t="n">
-        <v>0</v>
+        <v>-787585.1410615639</v>
       </c>
       <c r="V7" t="n">
-        <v>0</v>
+        <v>-2752.058173080708</v>
       </c>
       <c r="W7" t="n">
-        <v>0</v>
+        <v>-3653.751817487955</v>
       </c>
       <c r="X7" t="n">
-        <v>0</v>
+        <v>-743324.3819606152</v>
       </c>
       <c r="Y7" t="n">
-        <v>0</v>
+        <v>-1006998.176774388</v>
       </c>
       <c r="Z7" t="n">
-        <v>0</v>
+        <v>-4856080.747550545</v>
       </c>
       <c r="AA7" t="n">
-        <v>0</v>
+        <v>-5142181.816489385</v>
       </c>
       <c r="AB7" t="n">
-        <v>0</v>
+        <v>0.4400594123029106</v>
       </c>
       <c r="AC7" t="n">
-        <v>0</v>
+        <v>0.557875130341895</v>
       </c>
       <c r="AD7" t="n">
-        <v>0</v>
+        <v>0.002065457355194391</v>
       </c>
       <c r="AE7" t="n">
-        <v>0</v>
+        <v>0.4379762570534424</v>
       </c>
       <c r="AF7" t="n">
-        <v>0</v>
+        <v>0.5599918908180771</v>
       </c>
       <c r="AG7" t="n">
-        <v>0</v>
+        <v>0.002031852128480542</v>
       </c>
     </row>
     <row r="8">
@@ -1231,94 +1231,94 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>-20.93</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>-22.93</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>-63.13</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>1274540.934203486</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>-5581063.919999999</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>-3908551.920000001</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>40176</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>-1712688</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>-4306522.985796515</v>
       </c>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>-1054719.097866653</v>
       </c>
       <c r="S8" t="n">
-        <v>0</v>
+        <v>-1378468.870588656</v>
       </c>
       <c r="T8" t="n">
-        <v>0</v>
+        <v>-584641.2559666471</v>
       </c>
       <c r="U8" t="n">
-        <v>0</v>
+        <v>-785297.6196750915</v>
       </c>
       <c r="V8" t="n">
-        <v>0</v>
+        <v>-3046.921548767929</v>
       </c>
       <c r="W8" t="n">
-        <v>0</v>
+        <v>-4045.225226504521</v>
       </c>
       <c r="X8" t="n">
-        <v>0</v>
+        <v>-861489.2695434667</v>
       </c>
       <c r="Y8" t="n">
-        <v>0</v>
+        <v>-1166113.830774211</v>
       </c>
       <c r="Z8" t="n">
-        <v>0</v>
+        <v>-5361242.083663167</v>
       </c>
       <c r="AA8" t="n">
-        <v>0</v>
+        <v>-5684991.85638517</v>
       </c>
       <c r="AB8" t="n">
-        <v>0</v>
+        <v>0.4034297229460627</v>
       </c>
       <c r="AC8" t="n">
-        <v>0</v>
+        <v>0.5944677591359614</v>
       </c>
       <c r="AD8" t="n">
-        <v>0</v>
+        <v>0.002102517917975941</v>
       </c>
       <c r="AE8" t="n">
-        <v>0</v>
+        <v>0.4015929524000792</v>
       </c>
       <c r="AF8" t="n">
-        <v>0</v>
+        <v>0.5963383619180422</v>
       </c>
       <c r="AG8" t="n">
-        <v>0</v>
+        <v>0.002068685681878628</v>
       </c>
     </row>
     <row r="9">
@@ -1334,94 +1334,94 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>-19.41</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>-21.41</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>-62.21</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>33.1</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>975652.3105195034</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>-5143255.199999999</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>-3507775.199999999</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>38880</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>-1674360</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>-4167602.889480497</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>-1002203.489046597</v>
       </c>
       <c r="S9" t="n">
-        <v>0</v>
+        <v>-1314895.384586521</v>
       </c>
       <c r="T9" t="n">
-        <v>0</v>
+        <v>-524693.0680600157</v>
       </c>
       <c r="U9" t="n">
-        <v>0</v>
+        <v>-704774.4462136572</v>
       </c>
       <c r="V9" t="n">
-        <v>0</v>
+        <v>-2948.633756872184</v>
       </c>
       <c r="W9" t="n">
-        <v>0</v>
+        <v>-3914.734090165665</v>
       </c>
       <c r="X9" t="n">
-        <v>0</v>
+        <v>-844407.5592522034</v>
       </c>
       <c r="Y9" t="n">
-        <v>0</v>
+        <v>-1140255.6966918</v>
       </c>
       <c r="Z9" t="n">
-        <v>0</v>
+        <v>-5169806.378527095</v>
       </c>
       <c r="AA9" t="n">
-        <v>0</v>
+        <v>-5482498.274067018</v>
       </c>
       <c r="AB9" t="n">
-        <v>0</v>
+        <v>0.3824156194298581</v>
       </c>
       <c r="AC9" t="n">
-        <v>0</v>
+        <v>0.6154353077631096</v>
       </c>
       <c r="AD9" t="n">
-        <v>0</v>
+        <v>0.002149072807032182</v>
       </c>
       <c r="AE9" t="n">
-        <v>0</v>
+        <v>0.3811765591188717</v>
       </c>
       <c r="AF9" t="n">
-        <v>0</v>
+        <v>0.6167061608373193</v>
       </c>
       <c r="AG9" t="n">
-        <v>0</v>
+        <v>0.002117280043808971</v>
       </c>
     </row>
     <row r="10">
@@ -1437,94 +1437,94 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>-19.83000000000001</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>-21.83000000000001</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>-61.59</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>10.66</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>31.1</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>1022324.934203486</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>-5328847.920000001</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>-3703133.520000001</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>40176</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>-1665890.4</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>-4306522.985796515</v>
       </c>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>-1022076.122514607</v>
       </c>
       <c r="S10" t="n">
-        <v>0</v>
+        <v>-1333177.558487181</v>
       </c>
       <c r="T10" t="n">
-        <v>0</v>
+        <v>-553914.7685532076</v>
       </c>
       <c r="U10" t="n">
-        <v>0</v>
+        <v>-744025.4084164882</v>
       </c>
       <c r="V10" t="n">
-        <v>0</v>
+        <v>-3046.921548767929</v>
       </c>
       <c r="W10" t="n">
-        <v>0</v>
+        <v>-4045.225226504521</v>
       </c>
       <c r="X10" t="n">
-        <v>0</v>
+        <v>-841429.5613524489</v>
       </c>
       <c r="Y10" t="n">
-        <v>0</v>
+        <v>-1137708.340673366</v>
       </c>
       <c r="Z10" t="n">
-        <v>0</v>
+        <v>-5328599.108311122</v>
       </c>
       <c r="AA10" t="n">
-        <v>0</v>
+        <v>-5639700.544283696</v>
       </c>
       <c r="AB10" t="n">
-        <v>0</v>
+        <v>0.3961085768929816</v>
       </c>
       <c r="AC10" t="n">
-        <v>0</v>
+        <v>0.6017125468121338</v>
       </c>
       <c r="AD10" t="n">
-        <v>0</v>
+        <v>0.002178876294884509</v>
       </c>
       <c r="AE10" t="n">
-        <v>0</v>
+        <v>0.3945453939988994</v>
       </c>
       <c r="AF10" t="n">
-        <v>0</v>
+        <v>0.6033094843926836</v>
       </c>
       <c r="AG10" t="n">
-        <v>0</v>
+        <v>0.002145121608417028</v>
       </c>
     </row>
     <row r="11">
@@ -1540,94 +1540,94 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>-22</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>-61.32</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>11.42</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>29.9</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>987381.1105195042</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>-5154984</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>-3614400.000000002</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>38880</v>
       </c>
       <c r="P11" t="n">
-        <v>0</v>
+        <v>-1579464</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>-4167602.889480497</v>
       </c>
       <c r="R11" t="n">
-        <v>0</v>
+        <v>-982116.3397916914</v>
       </c>
       <c r="S11" t="n">
-        <v>0</v>
+        <v>-1279433.111516504</v>
       </c>
       <c r="T11" t="n">
-        <v>0</v>
+        <v>-540642.0072746131</v>
       </c>
       <c r="U11" t="n">
-        <v>0</v>
+        <v>-726197.2655472993</v>
       </c>
       <c r="V11" t="n">
-        <v>0</v>
+        <v>-2948.633756872184</v>
       </c>
       <c r="W11" t="n">
-        <v>0</v>
+        <v>-3914.734090165665</v>
       </c>
       <c r="X11" t="n">
-        <v>0</v>
+        <v>-804397.3357329989</v>
       </c>
       <c r="Y11" t="n">
-        <v>0</v>
+        <v>-1083398.54907433</v>
       </c>
       <c r="Z11" t="n">
-        <v>0</v>
+        <v>-5149719.229272189</v>
       </c>
       <c r="AA11" t="n">
-        <v>0</v>
+        <v>-5447036.000997001</v>
       </c>
       <c r="AB11" t="n">
-        <v>0</v>
+        <v>0.4010733156331944</v>
       </c>
       <c r="AC11" t="n">
-        <v>0</v>
+        <v>0.5967392510901752</v>
       </c>
       <c r="AD11" t="n">
-        <v>0</v>
+        <v>0.002187433276630299</v>
       </c>
       <c r="AE11" t="n">
-        <v>0</v>
+        <v>0.4004372988418207</v>
       </c>
       <c r="AF11" t="n">
-        <v>0</v>
+        <v>0.5974040514095211</v>
       </c>
       <c r="AG11" t="n">
-        <v>0</v>
+        <v>0.002158649748658175</v>
       </c>
     </row>
     <row r="12">
@@ -1643,94 +1643,94 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>-20.58</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>-22.58</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>-61.26</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>11.38</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>29.3</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>1100779.734203487</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>-5407302.72</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>-3843191.519999998</v>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>40176</v>
       </c>
       <c r="P12" t="n">
-        <v>0</v>
+        <v>-1604287.2</v>
       </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>-4306522.985796515</v>
       </c>
       <c r="R12" t="n">
-        <v>0</v>
+        <v>-1016482.538198965</v>
       </c>
       <c r="S12" t="n">
-        <v>0</v>
+        <v>-1319096.781620724</v>
       </c>
       <c r="T12" t="n">
-        <v>0</v>
+        <v>-574864.6463350996</v>
       </c>
       <c r="U12" t="n">
-        <v>0</v>
+        <v>-772165.5524564468</v>
       </c>
       <c r="V12" t="n">
-        <v>0</v>
+        <v>-3046.921548767929</v>
       </c>
       <c r="W12" t="n">
-        <v>0</v>
+        <v>-4045.225226504521</v>
       </c>
       <c r="X12" t="n">
-        <v>0</v>
+        <v>-819241.2385504454</v>
       </c>
       <c r="Y12" t="n">
-        <v>0</v>
+        <v>-1101354.10034739</v>
       </c>
       <c r="Z12" t="n">
-        <v>0</v>
+        <v>-5323005.523995481</v>
       </c>
       <c r="AA12" t="n">
-        <v>0</v>
+        <v>-5625619.767417239</v>
       </c>
       <c r="AB12" t="n">
-        <v>0</v>
+        <v>0.4114543832912717</v>
       </c>
       <c r="AC12" t="n">
-        <v>0</v>
+        <v>0.5863648090442154</v>
       </c>
       <c r="AD12" t="n">
-        <v>0</v>
+        <v>0.002180807664513094</v>
       </c>
       <c r="AE12" t="n">
-        <v>0</v>
+        <v>0.4112590523457633</v>
       </c>
       <c r="AF12" t="n">
-        <v>0</v>
+        <v>0.5865864414244717</v>
       </c>
       <c r="AG12" t="n">
-        <v>0</v>
+        <v>0.0021545062297651</v>
       </c>
     </row>
     <row r="13">
@@ -1746,94 +1746,94 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>-22.01</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>-24.01</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>-61.61</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>10.98</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>28.62</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>1327052.454203486</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>-5633575.440000001</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>-4110235.439999999</v>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
+        <v>40176</v>
       </c>
       <c r="P13" t="n">
-        <v>0</v>
+        <v>-1563516</v>
       </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>-4306522.985796515</v>
       </c>
       <c r="R13" t="n">
-        <v>0</v>
+        <v>-1023051.917997444</v>
       </c>
       <c r="S13" t="n">
-        <v>0</v>
+        <v>-1326132.249577541</v>
       </c>
       <c r="T13" t="n">
-        <v>0</v>
+        <v>-614809.0799725725</v>
       </c>
       <c r="U13" t="n">
-        <v>0</v>
+        <v>-825819.427092633</v>
       </c>
       <c r="V13" t="n">
-        <v>0</v>
+        <v>-3046.921548767929</v>
       </c>
       <c r="W13" t="n">
-        <v>0</v>
+        <v>-4045.225226504521</v>
       </c>
       <c r="X13" t="n">
-        <v>0</v>
+        <v>-796830.4018853962</v>
       </c>
       <c r="Y13" t="n">
-        <v>0</v>
+        <v>-1072695.713340885</v>
       </c>
       <c r="Z13" t="n">
-        <v>0</v>
+        <v>-5329574.903793959</v>
       </c>
       <c r="AA13" t="n">
-        <v>0</v>
+        <v>-5632655.235374056</v>
       </c>
       <c r="AB13" t="n">
-        <v>0</v>
+        <v>0.4345903646857972</v>
       </c>
       <c r="AC13" t="n">
-        <v>0</v>
+        <v>0.5632558565393234</v>
       </c>
       <c r="AD13" t="n">
-        <v>0</v>
+        <v>0.002153778774879416</v>
       </c>
       <c r="AE13" t="n">
-        <v>0</v>
+        <v>0.4340568856568952</v>
       </c>
       <c r="AF13" t="n">
-        <v>0</v>
+        <v>0.5638169136193232</v>
       </c>
       <c r="AG13" t="n">
-        <v>0</v>
+        <v>0.002126200723781598</v>
       </c>
     </row>
     <row r="14">
@@ -1849,94 +1849,94 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>-23.13</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>-25.13</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>-62.23</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>9.899999999999999</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>29.2</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>1484490.710519504</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>-5652093.6</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>-4180053.6</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>38880</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>-1510920</v>
       </c>
       <c r="Q14" t="n">
-        <v>0</v>
+        <v>-4167602.889480497</v>
       </c>
       <c r="R14" t="n">
-        <v>0</v>
+        <v>-1005797.190345592</v>
       </c>
       <c r="S14" t="n">
-        <v>0</v>
+        <v>-1302355.567795186</v>
       </c>
       <c r="T14" t="n">
-        <v>0</v>
+        <v>-625252.4814130915</v>
       </c>
       <c r="U14" t="n">
-        <v>0</v>
+        <v>-839847.1376054533</v>
       </c>
       <c r="V14" t="n">
-        <v>0</v>
+        <v>-2948.633756872184</v>
       </c>
       <c r="W14" t="n">
-        <v>0</v>
+        <v>-3914.734090165665</v>
       </c>
       <c r="X14" t="n">
-        <v>0</v>
+        <v>-763035.029017351</v>
       </c>
       <c r="Y14" t="n">
-        <v>0</v>
+        <v>-1031532.239447194</v>
       </c>
       <c r="Z14" t="n">
-        <v>0</v>
+        <v>-5173400.079826089</v>
       </c>
       <c r="AA14" t="n">
-        <v>0</v>
+        <v>-5469958.457275683</v>
       </c>
       <c r="AB14" t="n">
-        <v>0</v>
+        <v>0.4494222523080942</v>
       </c>
       <c r="AC14" t="n">
-        <v>0</v>
+        <v>0.5484583132815852</v>
       </c>
       <c r="AD14" t="n">
-        <v>0</v>
+        <v>0.002119434410320483</v>
       </c>
       <c r="AE14" t="n">
-        <v>0</v>
+        <v>0.4478482242412879</v>
       </c>
       <c r="AF14" t="n">
-        <v>0</v>
+        <v>0.5500642450258502</v>
       </c>
       <c r="AG14" t="n">
-        <v>0</v>
+        <v>0.002087530732861955</v>
       </c>
     </row>
     <row r="15">
@@ -1952,94 +1952,94 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>-23</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>-62.54</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>9.139999999999997</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>30.4</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>1543474.614203487</v>
       </c>
       <c r="M15" t="n">
-        <v>0</v>
+        <v>-5849997.6</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>-4295112</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>40176</v>
       </c>
       <c r="P15" t="n">
-        <v>0</v>
+        <v>-1595061.6</v>
       </c>
       <c r="Q15" t="n">
-        <v>0</v>
+        <v>-4306522.985796515</v>
       </c>
       <c r="R15" t="n">
-        <v>0</v>
+        <v>-1041464.877178975</v>
       </c>
       <c r="S15" t="n">
-        <v>0</v>
+        <v>-1358624.320554062</v>
       </c>
       <c r="T15" t="n">
-        <v>0</v>
+        <v>-642462.9186446676</v>
       </c>
       <c r="U15" t="n">
-        <v>0</v>
+        <v>-862964.4172253761</v>
       </c>
       <c r="V15" t="n">
-        <v>0</v>
+        <v>-3046.921548767929</v>
       </c>
       <c r="W15" t="n">
-        <v>0</v>
+        <v>-4045.225226504521</v>
       </c>
       <c r="X15" t="n">
-        <v>0</v>
+        <v>-806414.143289967</v>
       </c>
       <c r="Y15" t="n">
-        <v>0</v>
+        <v>-1086499.804170407</v>
       </c>
       <c r="Z15" t="n">
-        <v>0</v>
+        <v>-5347987.862975489</v>
       </c>
       <c r="AA15" t="n">
-        <v>0</v>
+        <v>-5665147.306350577</v>
       </c>
       <c r="AB15" t="n">
-        <v>0</v>
+        <v>0.4424907405298825</v>
       </c>
       <c r="AC15" t="n">
-        <v>0</v>
+        <v>0.5554107187865633</v>
       </c>
       <c r="AD15" t="n">
-        <v>0</v>
+        <v>0.002098540683554153</v>
       </c>
       <c r="AE15" t="n">
-        <v>0</v>
+        <v>0.4417508288570005</v>
       </c>
       <c r="AF15" t="n">
-        <v>0</v>
+        <v>0.5561784234261155</v>
       </c>
       <c r="AG15" t="n">
-        <v>0</v>
+        <v>0.002070747716884047</v>
       </c>
     </row>
     <row r="16">
@@ -2055,94 +2055,94 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>-21.48</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>-23.48</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>-62.5</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>9.219999999999999</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>31.8</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>1281486.710519504</v>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
+        <v>-5449089.6</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>-3881865.6</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>38880</v>
       </c>
       <c r="P16" t="n">
-        <v>0</v>
+        <v>-1606104</v>
       </c>
       <c r="Q16" t="n">
-        <v>0</v>
+        <v>-4167602.889480497</v>
       </c>
       <c r="R16" t="n">
-        <v>0</v>
+        <v>-1011281.612983699</v>
       </c>
       <c r="S16" t="n">
-        <v>0</v>
+        <v>-1316591.191231475</v>
       </c>
       <c r="T16" t="n">
-        <v>0</v>
+        <v>-580649.5158129368</v>
       </c>
       <c r="U16" t="n">
-        <v>0</v>
+        <v>-779935.8631978016</v>
       </c>
       <c r="V16" t="n">
-        <v>0</v>
+        <v>-2948.633756872184</v>
       </c>
       <c r="W16" t="n">
-        <v>0</v>
+        <v>-3914.734090165665</v>
       </c>
       <c r="X16" t="n">
-        <v>0</v>
+        <v>-810185.0517711509</v>
       </c>
       <c r="Y16" t="n">
-        <v>0</v>
+        <v>-1093695.788318272</v>
       </c>
       <c r="Z16" t="n">
-        <v>0</v>
+        <v>-5178884.502464197</v>
       </c>
       <c r="AA16" t="n">
-        <v>0</v>
+        <v>-5484194.080711972</v>
       </c>
       <c r="AB16" t="n">
-        <v>0</v>
+        <v>0.4165995940073703</v>
       </c>
       <c r="AC16" t="n">
-        <v>0</v>
+        <v>0.5812848447245391</v>
       </c>
       <c r="AD16" t="n">
-        <v>0</v>
+        <v>0.002115561268090547</v>
       </c>
       <c r="AE16" t="n">
-        <v>0</v>
+        <v>0.4154016482239766</v>
       </c>
       <c r="AF16" t="n">
-        <v>0</v>
+        <v>0.5825133252114724</v>
       </c>
       <c r="AG16" t="n">
-        <v>0</v>
+        <v>0.002085026564550969</v>
       </c>
     </row>
     <row r="17">
@@ -2158,94 +2158,94 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>-21.85</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>-23.85</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>-62.71</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>9.259999999999998</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>31.6</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>1385411.814203485</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>-5691934.800000001</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>-4080356.400000001</v>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>40176</v>
       </c>
       <c r="P17" t="n">
-        <v>0</v>
+        <v>-1651754.4</v>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>-4306522.985796515</v>
       </c>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>-1049181.700952156</v>
       </c>
       <c r="S17" t="n">
-        <v>0</v>
+        <v>-1363956.494863039</v>
       </c>
       <c r="T17" t="n">
-        <v>0</v>
+        <v>-610339.7727124341</v>
       </c>
       <c r="U17" t="n">
-        <v>0</v>
+        <v>-819816.1963641068</v>
       </c>
       <c r="V17" t="n">
-        <v>0</v>
+        <v>-3046.921548767929</v>
       </c>
       <c r="W17" t="n">
-        <v>0</v>
+        <v>-4045.225226504521</v>
       </c>
       <c r="X17" t="n">
-        <v>0</v>
+        <v>-833012.1535374742</v>
       </c>
       <c r="Y17" t="n">
-        <v>0</v>
+        <v>-1124860.688376899</v>
       </c>
       <c r="Z17" t="n">
-        <v>0</v>
+        <v>-5355704.68674867</v>
       </c>
       <c r="AA17" t="n">
-        <v>0</v>
+        <v>-5670479.480659554</v>
       </c>
       <c r="AB17" t="n">
-        <v>0</v>
+        <v>0.4219719710378164</v>
       </c>
       <c r="AC17" t="n">
-        <v>0</v>
+        <v>0.5759214720097875</v>
       </c>
       <c r="AD17" t="n">
-        <v>0</v>
+        <v>0.002106556952396044</v>
       </c>
       <c r="AE17" t="n">
-        <v>0</v>
+        <v>0.4206942550560865</v>
       </c>
       <c r="AF17" t="n">
-        <v>0</v>
+        <v>0.5772299101156362</v>
       </c>
       <c r="AG17" t="n">
-        <v>0</v>
+        <v>0.002075834828277267</v>
       </c>
     </row>
     <row r="18">
@@ -2261,94 +2261,94 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>6.549999999999997</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>-0.4500000000000028</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>-35.1</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>19.3</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>22.35</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>-3216942.72320749</v>
       </c>
       <c r="M18" t="n">
-        <v>0</v>
+        <v>476718</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>1023372</v>
       </c>
       <c r="O18" t="n">
-        <v>0</v>
+        <v>156240</v>
       </c>
       <c r="P18" t="n">
-        <v>0</v>
+        <v>-702894</v>
       </c>
       <c r="Q18" t="n">
-        <v>0</v>
+        <v>-2740224.723207489</v>
       </c>
       <c r="R18" t="n">
-        <v>0</v>
+        <v>-148219.0688156445</v>
       </c>
       <c r="S18" t="n">
-        <v>0</v>
+        <v>-189601.9794966906</v>
       </c>
       <c r="T18" t="n">
-        <v>0</v>
+        <v>-108372.2201245564</v>
       </c>
       <c r="U18" t="n">
-        <v>0</v>
+        <v>-143241.4030233921</v>
       </c>
       <c r="V18" t="n">
-        <v>0</v>
+        <v>-5400.630080600808</v>
       </c>
       <c r="W18" t="n">
-        <v>0</v>
+        <v>-7265.76732987675</v>
       </c>
       <c r="X18" t="n">
-        <v>0</v>
+        <v>-97790.13324254188</v>
       </c>
       <c r="Y18" t="n">
-        <v>0</v>
+        <v>-125256.557404092</v>
       </c>
       <c r="Z18" t="n">
-        <v>0</v>
+        <v>-2888443.792023133</v>
       </c>
       <c r="AA18" t="n">
-        <v>0</v>
+        <v>-2929826.70270418</v>
       </c>
       <c r="AB18" t="n">
-        <v>0</v>
+        <v>0.5122456601740414</v>
       </c>
       <c r="AC18" t="n">
-        <v>0</v>
+        <v>0.4622270477042918</v>
       </c>
       <c r="AD18" t="n">
-        <v>0</v>
+        <v>0.02552729212166697</v>
       </c>
       <c r="AE18" t="n">
-        <v>0</v>
+        <v>0.5194352578139915</v>
       </c>
       <c r="AF18" t="n">
-        <v>0</v>
+        <v>0.4542169429704794</v>
       </c>
       <c r="AG18" t="n">
-        <v>0</v>
+        <v>0.02634779921552901</v>
       </c>
     </row>
     <row r="19">
@@ -2364,94 +2364,94 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>672</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>4.760000000000005</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>-2.239999999999995</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>-35.48</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>18.54</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>21.7</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>-2674155.285477732</v>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>199113.6000000006</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>671731.2000000002</v>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>141120</v>
       </c>
       <c r="P19" t="n">
-        <v>0</v>
+        <v>-613737.6</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>-2475041.685477732</v>
       </c>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>-113188.8392099865</v>
       </c>
       <c r="S19" t="n">
-        <v>0</v>
+        <v>-143828.3342083992</v>
       </c>
       <c r="T19" t="n">
-        <v>0</v>
+        <v>-71134.44717163622</v>
       </c>
       <c r="U19" t="n">
-        <v>0</v>
+        <v>-94022.23193773735</v>
       </c>
       <c r="V19" t="n">
-        <v>0</v>
+        <v>-4877.988459897517</v>
       </c>
       <c r="W19" t="n">
-        <v>0</v>
+        <v>-6562.62855601771</v>
       </c>
       <c r="X19" t="n">
-        <v>0</v>
+        <v>-85465.31954207401</v>
       </c>
       <c r="Y19" t="n">
-        <v>0</v>
+        <v>-109472.8788420676</v>
       </c>
       <c r="Z19" t="n">
-        <v>0</v>
+        <v>-2588230.524687719</v>
       </c>
       <c r="AA19" t="n">
-        <v>0</v>
+        <v>-2618870.019686131</v>
       </c>
       <c r="AB19" t="n">
-        <v>0</v>
+        <v>0.4405216501502529</v>
       </c>
       <c r="AC19" t="n">
-        <v>0</v>
+        <v>0.5292699260662167</v>
       </c>
       <c r="AD19" t="n">
-        <v>0</v>
+        <v>0.03020842378353044</v>
       </c>
       <c r="AE19" t="n">
-        <v>0</v>
+        <v>0.4476018462115434</v>
       </c>
       <c r="AF19" t="n">
-        <v>0</v>
+        <v>0.5211561315865232</v>
       </c>
       <c r="AG19" t="n">
-        <v>0</v>
+        <v>0.03124202220193341</v>
       </c>
     </row>
     <row r="20">
@@ -2467,94 +2467,94 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>7.069999999999993</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>0.06999999999999318</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>-35.13</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>19.2</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="L20" t="n">
-        <v>0</v>
+        <v>-3287585.52320749</v>
       </c>
       <c r="M20" t="n">
-        <v>0</v>
+        <v>547360.7999999998</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>1104616.8</v>
       </c>
       <c r="O20" t="n">
-        <v>0</v>
+        <v>156240</v>
       </c>
       <c r="P20" t="n">
-        <v>0</v>
+        <v>-713496</v>
       </c>
       <c r="Q20" t="n">
-        <v>0</v>
+        <v>-2740224.723207489</v>
       </c>
       <c r="R20" t="n">
-        <v>0</v>
+        <v>-155559.3314618255</v>
       </c>
       <c r="S20" t="n">
-        <v>0</v>
+        <v>-199844.3551677452</v>
       </c>
       <c r="T20" t="n">
-        <v>0</v>
+        <v>-116975.8162260486</v>
       </c>
       <c r="U20" t="n">
-        <v>0</v>
+        <v>-154613.2395992957</v>
       </c>
       <c r="V20" t="n">
-        <v>0</v>
+        <v>-5400.630080600808</v>
       </c>
       <c r="W20" t="n">
-        <v>0</v>
+        <v>-7265.76732987675</v>
       </c>
       <c r="X20" t="n">
-        <v>0</v>
+        <v>-99649.14260457578</v>
       </c>
       <c r="Y20" t="n">
-        <v>0</v>
+        <v>-127540.8644923281</v>
       </c>
       <c r="Z20" t="n">
-        <v>0</v>
+        <v>-2895784.054669315</v>
       </c>
       <c r="AA20" t="n">
-        <v>0</v>
+        <v>-2940069.078375234</v>
       </c>
       <c r="AB20" t="n">
-        <v>0</v>
+        <v>0.5268573627016491</v>
       </c>
       <c r="AC20" t="n">
-        <v>0</v>
+        <v>0.4488182785292353</v>
       </c>
       <c r="AD20" t="n">
-        <v>0</v>
+        <v>0.02432435876911556</v>
       </c>
       <c r="AE20" t="n">
-        <v>0</v>
+        <v>0.5342177744738287</v>
       </c>
       <c r="AF20" t="n">
-        <v>0</v>
+        <v>0.4406776351115926</v>
       </c>
       <c r="AG20" t="n">
-        <v>0</v>
+        <v>0.02510459041457852</v>
       </c>
     </row>
     <row r="21">
@@ -2570,94 +2570,94 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>8.590000000000003</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>1.590000000000003</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>-34.21</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>19.7</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>23.1</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>-3402358.37729757</v>
       </c>
       <c r="M21" t="n">
-        <v>0</v>
+        <v>750528</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>1298808</v>
       </c>
       <c r="O21" t="n">
-        <v>0</v>
+        <v>151200</v>
       </c>
       <c r="P21" t="n">
-        <v>0</v>
+        <v>-699480</v>
       </c>
       <c r="Q21" t="n">
-        <v>0</v>
+        <v>-2651830.37729757</v>
       </c>
       <c r="R21" t="n">
-        <v>0</v>
+        <v>-169926.1680205621</v>
       </c>
       <c r="S21" t="n">
-        <v>0</v>
+        <v>-220248.5269172566</v>
       </c>
       <c r="T21" t="n">
-        <v>0</v>
+        <v>-137540.1188185076</v>
       </c>
       <c r="U21" t="n">
-        <v>0</v>
+        <v>-181794.1864522431</v>
       </c>
       <c r="V21" t="n">
-        <v>0</v>
+        <v>-5226.416207033062</v>
       </c>
       <c r="W21" t="n">
-        <v>0</v>
+        <v>-7031.387738590402</v>
       </c>
       <c r="X21" t="n">
-        <v>0</v>
+        <v>-97430.512632495</v>
       </c>
       <c r="Y21" t="n">
-        <v>0</v>
+        <v>-124787.4319188235</v>
       </c>
       <c r="Z21" t="n">
-        <v>0</v>
+        <v>-2821756.545318132</v>
       </c>
       <c r="AA21" t="n">
-        <v>0</v>
+        <v>-2872078.904214826</v>
       </c>
       <c r="AB21" t="n">
-        <v>0</v>
+        <v>0.5726136942961976</v>
       </c>
       <c r="AC21" t="n">
-        <v>0</v>
+        <v>0.4056274362339586</v>
       </c>
       <c r="AD21" t="n">
-        <v>0</v>
+        <v>0.02175886946984385</v>
       </c>
       <c r="AE21" t="n">
-        <v>0</v>
+        <v>0.5796768083931998</v>
       </c>
       <c r="AF21" t="n">
-        <v>0</v>
+        <v>0.3979026044448893</v>
       </c>
       <c r="AG21" t="n">
-        <v>0</v>
+        <v>0.02242058716191071</v>
       </c>
     </row>
     <row r="22">
@@ -2673,94 +2673,94 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>8.169999999999995</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>1.169999999999995</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>-33.59</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>20.66</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>21.1</v>
       </c>
       <c r="L22" t="n">
-        <v>0</v>
+        <v>-3473064.723207491</v>
       </c>
       <c r="M22" t="n">
-        <v>0</v>
+        <v>732840</v>
       </c>
       <c r="N22" t="n">
-        <v>0</v>
+        <v>1276480.800000001</v>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>156240</v>
       </c>
       <c r="P22" t="n">
-        <v>0</v>
+        <v>-699880.8</v>
       </c>
       <c r="Q22" t="n">
-        <v>0</v>
+        <v>-2740224.723207489</v>
       </c>
       <c r="R22" t="n">
-        <v>0</v>
+        <v>-167755.1129257497</v>
       </c>
       <c r="S22" t="n">
-        <v>0</v>
+        <v>-216999.9855145325</v>
       </c>
       <c r="T22" t="n">
-        <v>0</v>
+        <v>-135175.7310561275</v>
       </c>
       <c r="U22" t="n">
-        <v>0</v>
+        <v>-178669.0477406293</v>
       </c>
       <c r="V22" t="n">
-        <v>0</v>
+        <v>-5400.630080600808</v>
       </c>
       <c r="W22" t="n">
-        <v>0</v>
+        <v>-7265.76732987675</v>
       </c>
       <c r="X22" t="n">
-        <v>0</v>
+        <v>-96545.10966490401</v>
       </c>
       <c r="Y22" t="n">
-        <v>0</v>
+        <v>-123572.2124713685</v>
       </c>
       <c r="Z22" t="n">
-        <v>0</v>
+        <v>-2907979.836133239</v>
       </c>
       <c r="AA22" t="n">
-        <v>0</v>
+        <v>-2957224.708722021</v>
       </c>
       <c r="AB22" t="n">
-        <v>0</v>
+        <v>0.5700695537993304</v>
       </c>
       <c r="AC22" t="n">
-        <v>0</v>
+        <v>0.4071546508990337</v>
       </c>
       <c r="AD22" t="n">
-        <v>0</v>
+        <v>0.02277579530163589</v>
       </c>
       <c r="AE22" t="n">
-        <v>0</v>
+        <v>0.5772697607535143</v>
       </c>
       <c r="AF22" t="n">
-        <v>0</v>
+        <v>0.3992549489192128</v>
       </c>
       <c r="AG22" t="n">
-        <v>0</v>
+        <v>0.02347529032727288</v>
       </c>
     </row>
     <row r="23">
@@ -2776,94 +2776,94 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>-33.32</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>21.42</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>19.9</v>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
+        <v>-3345982.37729757</v>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>694152</v>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>1209600</v>
       </c>
       <c r="O23" t="n">
-        <v>0</v>
+        <v>151200</v>
       </c>
       <c r="P23" t="n">
-        <v>0</v>
+        <v>-666648</v>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
+        <v>-2651830.37729757</v>
       </c>
       <c r="R23" t="n">
-        <v>0</v>
+        <v>-159538.9990451986</v>
       </c>
       <c r="S23" t="n">
-        <v>0</v>
+        <v>-205720.9652579391</v>
       </c>
       <c r="T23" t="n">
-        <v>0</v>
+        <v>-128093.2422058283</v>
       </c>
       <c r="U23" t="n">
-        <v>0</v>
+        <v>-169307.7405841616</v>
       </c>
       <c r="V23" t="n">
-        <v>0</v>
+        <v>-5226.416207033062</v>
       </c>
       <c r="W23" t="n">
-        <v>0</v>
+        <v>-7031.387738590402</v>
       </c>
       <c r="X23" t="n">
-        <v>0</v>
+        <v>-91387.29659903797</v>
       </c>
       <c r="Y23" t="n">
-        <v>0</v>
+        <v>-117210.8447177584</v>
       </c>
       <c r="Z23" t="n">
-        <v>0</v>
+        <v>-2811369.376342769</v>
       </c>
       <c r="AA23" t="n">
-        <v>0</v>
+        <v>-2857551.342555509</v>
       </c>
       <c r="AB23" t="n">
-        <v>0</v>
+        <v>0.5700457389004498</v>
       </c>
       <c r="AC23" t="n">
-        <v>0</v>
+        <v>0.4066954518350291</v>
       </c>
       <c r="AD23" t="n">
-        <v>0</v>
+        <v>0.02325880926452097</v>
       </c>
       <c r="AE23" t="n">
-        <v>0</v>
+        <v>0.5767595167205034</v>
       </c>
       <c r="AF23" t="n">
-        <v>0</v>
+        <v>0.399287533579787</v>
       </c>
       <c r="AG23" t="n">
-        <v>0</v>
+        <v>0.02395294969970941</v>
       </c>
     </row>
     <row r="24">
@@ -2879,94 +2879,94 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>7.420000000000002</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>0.4200000000000017</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>-33.26</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>0</v>
+        <v>21.38</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>19.3</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>-3378651.123207489</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>638426.3999999994</v>
       </c>
       <c r="N24" t="n">
-        <v>0</v>
+        <v>1159300.8</v>
       </c>
       <c r="O24" t="n">
-        <v>0</v>
+        <v>156240</v>
       </c>
       <c r="P24" t="n">
-        <v>0</v>
+        <v>-677114.4</v>
       </c>
       <c r="Q24" t="n">
-        <v>0</v>
+        <v>-2740224.723207489</v>
       </c>
       <c r="R24" t="n">
-        <v>0</v>
+        <v>-156123.5865061626</v>
       </c>
       <c r="S24" t="n">
-        <v>0</v>
+        <v>-200951.8306462598</v>
       </c>
       <c r="T24" t="n">
-        <v>0</v>
+        <v>-122766.6982174359</v>
       </c>
       <c r="U24" t="n">
-        <v>0</v>
+        <v>-162267.3603715367</v>
       </c>
       <c r="V24" t="n">
-        <v>0</v>
+        <v>-5400.630080600808</v>
       </c>
       <c r="W24" t="n">
-        <v>0</v>
+        <v>-7265.76732987675</v>
       </c>
       <c r="X24" t="n">
-        <v>0</v>
+        <v>-93009.4370855178</v>
       </c>
       <c r="Y24" t="n">
-        <v>0</v>
+        <v>-118957.3373572592</v>
       </c>
       <c r="Z24" t="n">
-        <v>0</v>
+        <v>-2896348.309713652</v>
       </c>
       <c r="AA24" t="n">
-        <v>0</v>
+        <v>-2941176.553853749</v>
       </c>
       <c r="AB24" t="n">
-        <v>0</v>
+        <v>0.5550614595730232</v>
       </c>
       <c r="AC24" t="n">
-        <v>0</v>
+        <v>0.420520830586455</v>
       </c>
       <c r="AD24" t="n">
-        <v>0</v>
+        <v>0.02441770984052184</v>
       </c>
       <c r="AE24" t="n">
-        <v>0</v>
+        <v>0.5624704453872855</v>
       </c>
       <c r="AF24" t="n">
-        <v>0</v>
+        <v>0.4123440867727321</v>
       </c>
       <c r="AG24" t="n">
-        <v>0</v>
+        <v>0.02518546783998234</v>
       </c>
     </row>
     <row r="25">
@@ -2982,94 +2982,94 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>5.990000000000002</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>-1.009999999999998</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>-33.61</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>20.98</v>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>18.62</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>-3173827.92320749</v>
       </c>
       <c r="M25" t="n">
-        <v>0</v>
+        <v>433603.1999999993</v>
       </c>
       <c r="N25" t="n">
-        <v>0</v>
+        <v>935877.5999999996</v>
       </c>
       <c r="O25" t="n">
-        <v>0</v>
+        <v>156240</v>
       </c>
       <c r="P25" t="n">
-        <v>0</v>
+        <v>-658514.4</v>
       </c>
       <c r="Q25" t="n">
-        <v>0</v>
+        <v>-2740224.723207489</v>
       </c>
       <c r="R25" t="n">
-        <v>0</v>
+        <v>-136623.7626294145</v>
       </c>
       <c r="S25" t="n">
-        <v>0</v>
+        <v>-174281.2715486164</v>
       </c>
       <c r="T25" t="n">
-        <v>0</v>
+        <v>-99106.80893833385</v>
       </c>
       <c r="U25" t="n">
-        <v>0</v>
+        <v>-130994.8097878035</v>
       </c>
       <c r="V25" t="n">
-        <v>0</v>
+        <v>-5400.630080600808</v>
       </c>
       <c r="W25" t="n">
-        <v>0</v>
+        <v>-7265.76732987675</v>
       </c>
       <c r="X25" t="n">
-        <v>0</v>
+        <v>-90570.94819218389</v>
       </c>
       <c r="Y25" t="n">
-        <v>0</v>
+        <v>-115657.7193760295</v>
       </c>
       <c r="Z25" t="n">
-        <v>0</v>
+        <v>-2876848.485836904</v>
       </c>
       <c r="AA25" t="n">
-        <v>0</v>
+        <v>-2914505.994756105</v>
       </c>
       <c r="AB25" t="n">
-        <v>0</v>
+        <v>0.5080358227027891</v>
       </c>
       <c r="AC25" t="n">
-        <v>0</v>
+        <v>0.4642797671592693</v>
       </c>
       <c r="AD25" t="n">
-        <v>0</v>
+        <v>0.02768441013794171</v>
       </c>
       <c r="AE25" t="n">
-        <v>0</v>
+        <v>0.5158935436976224</v>
       </c>
       <c r="AF25" t="n">
-        <v>0</v>
+        <v>0.4554918687354012</v>
       </c>
       <c r="AG25" t="n">
-        <v>0</v>
+        <v>0.02861458756697647</v>
       </c>
     </row>
     <row r="26">
@@ -3085,94 +3085,94 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>4.870000000000005</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>-2.129999999999995</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>-34.23</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>0</v>
+        <v>19.9</v>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>19.2</v>
       </c>
       <c r="L26" t="n">
-        <v>0</v>
+        <v>-2907214.37729757</v>
       </c>
       <c r="M26" t="n">
-        <v>0</v>
+        <v>255384</v>
       </c>
       <c r="N26" t="n">
-        <v>0</v>
+        <v>736344</v>
       </c>
       <c r="O26" t="n">
-        <v>0</v>
+        <v>151200</v>
       </c>
       <c r="P26" t="n">
-        <v>0</v>
+        <v>-632160</v>
       </c>
       <c r="Q26" t="n">
-        <v>0</v>
+        <v>-2651830.37729757</v>
       </c>
       <c r="R26" t="n">
-        <v>0</v>
+        <v>-118137.791694634</v>
       </c>
       <c r="S26" t="n">
-        <v>0</v>
+        <v>-151117.5627034196</v>
       </c>
       <c r="T26" t="n">
-        <v>0</v>
+        <v>-77976.76119279733</v>
       </c>
       <c r="U26" t="n">
-        <v>0</v>
+        <v>-103066.0870806077</v>
       </c>
       <c r="V26" t="n">
-        <v>0</v>
+        <v>-5226.416207033062</v>
       </c>
       <c r="W26" t="n">
-        <v>0</v>
+        <v>-7031.387738590402</v>
       </c>
       <c r="X26" t="n">
-        <v>0</v>
+        <v>-86934.92239554616</v>
       </c>
       <c r="Y26" t="n">
-        <v>0</v>
+        <v>-111301.0763857183</v>
       </c>
       <c r="Z26" t="n">
-        <v>0</v>
+        <v>-2769968.168992204</v>
       </c>
       <c r="AA26" t="n">
-        <v>0</v>
+        <v>-2802947.940000989</v>
       </c>
       <c r="AB26" t="n">
-        <v>0</v>
+        <v>0.4583145179508836</v>
       </c>
       <c r="AC26" t="n">
-        <v>0</v>
+        <v>0.5109668116671219</v>
       </c>
       <c r="AD26" t="n">
-        <v>0</v>
+        <v>0.03071867038199452</v>
       </c>
       <c r="AE26" t="n">
-        <v>0</v>
+        <v>0.4655228614626951</v>
       </c>
       <c r="AF26" t="n">
-        <v>0</v>
+        <v>0.502718178506521</v>
       </c>
       <c r="AG26" t="n">
-        <v>0</v>
+        <v>0.03175896003078389</v>
       </c>
     </row>
     <row r="27">
@@ -3188,94 +3188,94 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>-34.54</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>19.14</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>20.4</v>
       </c>
       <c r="L27" t="n">
-        <v>0</v>
+        <v>-3013421.52320749</v>
       </c>
       <c r="M27" t="n">
-        <v>0</v>
+        <v>273196.8000000007</v>
       </c>
       <c r="N27" t="n">
-        <v>0</v>
+        <v>781200</v>
       </c>
       <c r="O27" t="n">
-        <v>0</v>
+        <v>156240</v>
       </c>
       <c r="P27" t="n">
-        <v>0</v>
+        <v>-664243.2</v>
       </c>
       <c r="Q27" t="n">
-        <v>0</v>
+        <v>-2740224.723207489</v>
       </c>
       <c r="R27" t="n">
-        <v>0</v>
+        <v>-125663.0360709857</v>
       </c>
       <c r="S27" t="n">
-        <v>0</v>
+        <v>-159978.9580795815</v>
       </c>
       <c r="T27" t="n">
-        <v>0</v>
+        <v>-82726.88559126419</v>
       </c>
       <c r="U27" t="n">
-        <v>0</v>
+        <v>-109344.5824606044</v>
       </c>
       <c r="V27" t="n">
-        <v>0</v>
+        <v>-5400.630080600808</v>
       </c>
       <c r="W27" t="n">
-        <v>0</v>
+        <v>-7265.76732987675</v>
       </c>
       <c r="X27" t="n">
-        <v>0</v>
+        <v>-91965.7695767407</v>
       </c>
       <c r="Y27" t="n">
-        <v>0</v>
+        <v>-117594.7395266114</v>
       </c>
       <c r="Z27" t="n">
-        <v>0</v>
+        <v>-2865887.759278475</v>
       </c>
       <c r="AA27" t="n">
-        <v>0</v>
+        <v>-2900203.681287071</v>
       </c>
       <c r="AB27" t="n">
-        <v>0</v>
+        <v>0.4593557470899913</v>
       </c>
       <c r="AC27" t="n">
-        <v>0</v>
+        <v>0.5106562937634717</v>
       </c>
       <c r="AD27" t="n">
-        <v>0</v>
+        <v>0.02998795914653692</v>
       </c>
       <c r="AE27" t="n">
-        <v>0</v>
+        <v>0.4668753474975161</v>
       </c>
       <c r="AF27" t="n">
-        <v>0</v>
+        <v>0.5021015549640715</v>
       </c>
       <c r="AG27" t="n">
-        <v>0</v>
+        <v>0.0310230975384124</v>
       </c>
     </row>
     <row r="28">
@@ -3291,94 +3291,94 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>6.519999999999996</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>-0.480000000000004</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>-34.5</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>0</v>
+        <v>19.22</v>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>21.8</v>
       </c>
       <c r="L28" t="n">
-        <v>0</v>
+        <v>-3119686.37729757</v>
       </c>
       <c r="M28" t="n">
-        <v>0</v>
+        <v>467856</v>
       </c>
       <c r="N28" t="n">
-        <v>0</v>
+        <v>985824</v>
       </c>
       <c r="O28" t="n">
-        <v>0</v>
+        <v>151200</v>
       </c>
       <c r="P28" t="n">
-        <v>0</v>
+        <v>-669168</v>
       </c>
       <c r="Q28" t="n">
-        <v>0</v>
+        <v>-2651830.37729757</v>
       </c>
       <c r="R28" t="n">
-        <v>0</v>
+        <v>-141865.1092076128</v>
       </c>
       <c r="S28" t="n">
-        <v>0</v>
+        <v>-181630.39647501</v>
       </c>
       <c r="T28" t="n">
-        <v>0</v>
+        <v>-104395.9923977508</v>
       </c>
       <c r="U28" t="n">
-        <v>0</v>
+        <v>-137985.8085760923</v>
       </c>
       <c r="V28" t="n">
-        <v>0</v>
+        <v>-5226.416207033062</v>
       </c>
       <c r="W28" t="n">
-        <v>0</v>
+        <v>-7031.387738590402</v>
       </c>
       <c r="X28" t="n">
-        <v>0</v>
+        <v>-92828.8664102528</v>
       </c>
       <c r="Y28" t="n">
-        <v>0</v>
+        <v>-119033.915488946</v>
       </c>
       <c r="Z28" t="n">
-        <v>0</v>
+        <v>-2793695.486505183</v>
       </c>
       <c r="AA28" t="n">
-        <v>0</v>
+        <v>-2833460.77377258</v>
       </c>
       <c r="AB28" t="n">
-        <v>0</v>
+        <v>0.5156598415593924</v>
       </c>
       <c r="AC28" t="n">
-        <v>0</v>
+        <v>0.4585244839942753</v>
       </c>
       <c r="AD28" t="n">
-        <v>0</v>
+        <v>0.02581567444633224</v>
       </c>
       <c r="AE28" t="n">
-        <v>0</v>
+        <v>0.5225723445493783</v>
       </c>
       <c r="AF28" t="n">
-        <v>0</v>
+        <v>0.4507987664807485</v>
       </c>
       <c r="AG28" t="n">
-        <v>0</v>
+        <v>0.02662888896987319</v>
       </c>
     </row>
     <row r="29">
@@ -3394,94 +3394,94 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>6.149999999999999</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>-0.8500000000000014</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>-34.71</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>19.26</v>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>21.6</v>
       </c>
       <c r="L29" t="n">
-        <v>0</v>
+        <v>-3168991.923207491</v>
       </c>
       <c r="M29" t="n">
-        <v>0</v>
+        <v>428767.1999999993</v>
       </c>
       <c r="N29" t="n">
-        <v>0</v>
+        <v>960875.9999999981</v>
       </c>
       <c r="O29" t="n">
-        <v>0</v>
+        <v>156240</v>
       </c>
       <c r="P29" t="n">
-        <v>0</v>
+        <v>-688348.8</v>
       </c>
       <c r="Q29" t="n">
-        <v>0</v>
+        <v>-2740224.723207489</v>
       </c>
       <c r="R29" t="n">
-        <v>0</v>
+        <v>-140727.3984471318</v>
       </c>
       <c r="S29" t="n">
-        <v>0</v>
+        <v>-181080.1421427437</v>
       </c>
       <c r="T29" t="n">
-        <v>0</v>
+        <v>-101754.0692772533</v>
       </c>
       <c r="U29" t="n">
-        <v>0</v>
+        <v>-134493.8364265418</v>
       </c>
       <c r="V29" t="n">
-        <v>0</v>
+        <v>-5400.630080600808</v>
       </c>
       <c r="W29" t="n">
-        <v>0</v>
+        <v>-7265.76732987675</v>
       </c>
       <c r="X29" t="n">
-        <v>0</v>
+        <v>-95445.88971423659</v>
       </c>
       <c r="Y29" t="n">
-        <v>0</v>
+        <v>-122331.7084078602</v>
       </c>
       <c r="Z29" t="n">
-        <v>0</v>
+        <v>-2880952.121654621</v>
       </c>
       <c r="AA29" t="n">
-        <v>0</v>
+        <v>-2921304.865350233</v>
       </c>
       <c r="AB29" t="n">
-        <v>0</v>
+        <v>0.5022397503545584</v>
       </c>
       <c r="AC29" t="n">
-        <v>0</v>
+        <v>0.471103712735378</v>
       </c>
       <c r="AD29" t="n">
-        <v>0</v>
+        <v>0.02665653691006357</v>
       </c>
       <c r="AE29" t="n">
-        <v>0</v>
+        <v>0.5092702040227645</v>
       </c>
       <c r="AF29" t="n">
-        <v>0</v>
+        <v>0.4632174659792042</v>
       </c>
       <c r="AG29" t="n">
-        <v>0</v>
+        <v>0.02751232999803136</v>
       </c>
     </row>
     <row r="30">
@@ -3497,94 +3497,94 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>6.549999999999997</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>-0.4500000000000028</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>-35.1</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>19.3</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>22.35</v>
       </c>
       <c r="L30" t="n">
-        <v>0</v>
+        <v>-3773297.028858003</v>
       </c>
       <c r="M30" t="n">
-        <v>0</v>
+        <v>684591.5999999996</v>
       </c>
       <c r="N30" t="n">
-        <v>0</v>
+        <v>916161.5999999996</v>
       </c>
       <c r="O30" t="n">
-        <v>0</v>
+        <v>161448</v>
       </c>
       <c r="P30" t="n">
-        <v>0</v>
+        <v>-393018</v>
       </c>
       <c r="Q30" t="n">
-        <v>0</v>
+        <v>-3088705.428858003</v>
       </c>
       <c r="R30" t="n">
-        <v>0</v>
+        <v>-84778.06850604535</v>
       </c>
       <c r="S30" t="n">
-        <v>0</v>
+        <v>-107775.8812581551</v>
       </c>
       <c r="T30" t="n">
-        <v>0</v>
+        <v>-64266.47539554364</v>
       </c>
       <c r="U30" t="n">
-        <v>0</v>
+        <v>-85253.55558068701</v>
       </c>
       <c r="V30" t="n">
-        <v>0</v>
+        <v>-4586.264557766881</v>
       </c>
       <c r="W30" t="n">
-        <v>0</v>
+        <v>-5981.384428674952</v>
       </c>
       <c r="X30" t="n">
-        <v>0</v>
+        <v>-52695.14867557693</v>
       </c>
       <c r="Y30" t="n">
-        <v>0</v>
+        <v>-66877.08670172787</v>
       </c>
       <c r="Z30" t="n">
-        <v>0</v>
+        <v>-3173483.497364048</v>
       </c>
       <c r="AA30" t="n">
-        <v>0</v>
+        <v>-3196481.310116158</v>
       </c>
       <c r="AB30" t="n">
-        <v>0</v>
+        <v>0.5287337864976279</v>
       </c>
       <c r="AC30" t="n">
-        <v>0</v>
+        <v>0.4335340520514253</v>
       </c>
       <c r="AD30" t="n">
-        <v>0</v>
+        <v>0.03773216145094679</v>
       </c>
       <c r="AE30" t="n">
-        <v>0</v>
+        <v>0.53919715883768</v>
       </c>
       <c r="AF30" t="n">
-        <v>0</v>
+        <v>0.4229728003166325</v>
       </c>
       <c r="AG30" t="n">
-        <v>0</v>
+        <v>0.03783004084568744</v>
       </c>
     </row>
     <row r="31">
@@ -3600,94 +3600,94 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>696</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>4.760000000000005</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>-2.239999999999995</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>-35.48</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>18.54</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>21.7</v>
       </c>
       <c r="L31" t="n">
-        <v>0</v>
+        <v>-3307716.190867164</v>
       </c>
       <c r="M31" t="n">
-        <v>0</v>
+        <v>418282.0799999991</v>
       </c>
       <c r="N31" t="n">
-        <v>0</v>
+        <v>622836.4800000004</v>
       </c>
       <c r="O31" t="n">
-        <v>0</v>
+        <v>151032</v>
       </c>
       <c r="P31" t="n">
-        <v>0</v>
+        <v>-355586.4</v>
       </c>
       <c r="Q31" t="n">
-        <v>0</v>
+        <v>-2889434.110867164</v>
       </c>
       <c r="R31" t="n">
-        <v>0</v>
+        <v>-65668.83623777081</v>
       </c>
       <c r="S31" t="n">
-        <v>0</v>
+        <v>-83368.56786865566</v>
       </c>
       <c r="T31" t="n">
-        <v>0</v>
+        <v>-43690.44207633984</v>
       </c>
       <c r="U31" t="n">
-        <v>0</v>
+        <v>-57958.14239033738</v>
       </c>
       <c r="V31" t="n">
-        <v>0</v>
+        <v>-4290.376521781912</v>
       </c>
       <c r="W31" t="n">
-        <v>0</v>
+        <v>-5595.48865908302</v>
       </c>
       <c r="X31" t="n">
-        <v>0</v>
+        <v>-47756.96338970204</v>
       </c>
       <c r="Y31" t="n">
-        <v>0</v>
+        <v>-60597.16761279778</v>
       </c>
       <c r="Z31" t="n">
-        <v>0</v>
+        <v>-2955102.947104935</v>
       </c>
       <c r="AA31" t="n">
-        <v>0</v>
+        <v>-2972802.67873582</v>
       </c>
       <c r="AB31" t="n">
-        <v>0</v>
+        <v>0.4563552776049953</v>
       </c>
       <c r="AC31" t="n">
-        <v>0</v>
+        <v>0.498830894116347</v>
       </c>
       <c r="AD31" t="n">
-        <v>0</v>
+        <v>0.04481382827865778</v>
       </c>
       <c r="AE31" t="n">
-        <v>0</v>
+        <v>0.4668366455541403</v>
       </c>
       <c r="AF31" t="n">
-        <v>0</v>
+        <v>0.4880932564732573</v>
       </c>
       <c r="AG31" t="n">
-        <v>0</v>
+        <v>0.0450700979726025</v>
       </c>
     </row>
     <row r="32">
@@ -3703,94 +3703,94 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>7.069999999999993</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>0.06999999999999318</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>-35.13</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>19.2</v>
       </c>
       <c r="K32" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="L32" t="n">
-        <v>0</v>
+        <v>-3839520.468858003</v>
       </c>
       <c r="M32" t="n">
-        <v>0</v>
+        <v>750815.0399999991</v>
       </c>
       <c r="N32" t="n">
-        <v>0</v>
+        <v>988895.0399999991</v>
       </c>
       <c r="O32" t="n">
-        <v>0</v>
+        <v>161448</v>
       </c>
       <c r="P32" t="n">
-        <v>0</v>
+        <v>-399528</v>
       </c>
       <c r="Q32" t="n">
-        <v>0</v>
+        <v>-3088705.428858003</v>
       </c>
       <c r="R32" t="n">
-        <v>0</v>
+        <v>-89333.96131535592</v>
       </c>
       <c r="S32" t="n">
-        <v>0</v>
+        <v>-113993.297582964</v>
       </c>
       <c r="T32" t="n">
-        <v>0</v>
+        <v>-69368.54672465556</v>
       </c>
       <c r="U32" t="n">
-        <v>0</v>
+        <v>-92021.77678709278</v>
       </c>
       <c r="V32" t="n">
-        <v>0</v>
+        <v>-4586.264557766881</v>
       </c>
       <c r="W32" t="n">
-        <v>0</v>
+        <v>-5981.384428674952</v>
       </c>
       <c r="X32" t="n">
-        <v>0</v>
+        <v>-53769.88768742914</v>
       </c>
       <c r="Y32" t="n">
-        <v>0</v>
+        <v>-68308.01020931349</v>
       </c>
       <c r="Z32" t="n">
-        <v>0</v>
+        <v>-3178039.390173359</v>
       </c>
       <c r="AA32" t="n">
-        <v>0</v>
+        <v>-3202698.726440967</v>
       </c>
       <c r="AB32" t="n">
-        <v>0</v>
+        <v>0.5431098862173046</v>
       </c>
       <c r="AC32" t="n">
-        <v>0</v>
+        <v>0.4209826926280023</v>
       </c>
       <c r="AD32" t="n">
-        <v>0</v>
+        <v>0.03590742115469329</v>
       </c>
       <c r="AE32" t="n">
-        <v>0</v>
+        <v>0.5533108569832073</v>
       </c>
       <c r="AF32" t="n">
-        <v>0</v>
+        <v>0.4107241240861829</v>
       </c>
       <c r="AG32" t="n">
-        <v>0</v>
+        <v>0.03596501893060989</v>
       </c>
     </row>
     <row r="33">
@@ -3806,94 +3806,94 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>8.590000000000003</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>1.590000000000003</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>-34.21</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>0</v>
+        <v>19.7</v>
       </c>
       <c r="K33" t="n">
-        <v>0</v>
+        <v>23.1</v>
       </c>
       <c r="L33" t="n">
-        <v>0</v>
+        <v>-3916732.169862583</v>
       </c>
       <c r="M33" t="n">
-        <v>0</v>
+        <v>927662.4000000004</v>
       </c>
       <c r="N33" t="n">
-        <v>0</v>
+        <v>1162742.4</v>
       </c>
       <c r="O33" t="n">
-        <v>0</v>
+        <v>156240</v>
       </c>
       <c r="P33" t="n">
-        <v>0</v>
+        <v>-391320</v>
       </c>
       <c r="Q33" t="n">
-        <v>0</v>
+        <v>-2989069.769862582</v>
       </c>
       <c r="R33" t="n">
-        <v>0</v>
+        <v>-97880.06216377577</v>
       </c>
       <c r="S33" t="n">
-        <v>0</v>
+        <v>-126479.6461452728</v>
       </c>
       <c r="T33" t="n">
-        <v>0</v>
+        <v>-81563.51001936202</v>
       </c>
       <c r="U33" t="n">
-        <v>0</v>
+        <v>-108199.1690378869</v>
       </c>
       <c r="V33" t="n">
-        <v>0</v>
+        <v>-4438.320539774383</v>
       </c>
       <c r="W33" t="n">
-        <v>0</v>
+        <v>-5788.436543878986</v>
       </c>
       <c r="X33" t="n">
-        <v>0</v>
+        <v>-52530.1304260085</v>
       </c>
       <c r="Y33" t="n">
-        <v>0</v>
+        <v>-66703.80274329866</v>
       </c>
       <c r="Z33" t="n">
-        <v>0</v>
+        <v>-3086949.832026358</v>
       </c>
       <c r="AA33" t="n">
-        <v>0</v>
+        <v>-3115549.416007855</v>
       </c>
       <c r="AB33" t="n">
-        <v>0</v>
+        <v>0.5887703417993791</v>
       </c>
       <c r="AC33" t="n">
-        <v>0</v>
+        <v>0.3791914158469281</v>
       </c>
       <c r="AD33" t="n">
-        <v>0</v>
+        <v>0.03203824235369277</v>
       </c>
       <c r="AE33" t="n">
-        <v>0</v>
+        <v>0.5988063851007026</v>
       </c>
       <c r="AF33" t="n">
-        <v>0</v>
+        <v>0.3691586853056027</v>
       </c>
       <c r="AG33" t="n">
-        <v>0</v>
+        <v>0.03203492959369472</v>
       </c>
     </row>
     <row r="34">
@@ -3909,94 +3909,94 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>8.169999999999995</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>1.169999999999995</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>-33.59</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>20.66</v>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>21.1</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>-4003721.268858002</v>
       </c>
       <c r="M34" t="n">
-        <v>0</v>
+        <v>915015.8399999999</v>
       </c>
       <c r="N34" t="n">
-        <v>0</v>
+        <v>1142754.239999999</v>
       </c>
       <c r="O34" t="n">
-        <v>0</v>
+        <v>161448</v>
       </c>
       <c r="P34" t="n">
-        <v>0</v>
+        <v>-389186.4</v>
       </c>
       <c r="Q34" t="n">
-        <v>0</v>
+        <v>-3088705.428858003</v>
       </c>
       <c r="R34" t="n">
-        <v>0</v>
+        <v>-96086.83532006976</v>
       </c>
       <c r="S34" t="n">
-        <v>0</v>
+        <v>-124174.7100594716</v>
       </c>
       <c r="T34" t="n">
-        <v>0</v>
+        <v>-80161.38992085353</v>
       </c>
       <c r="U34" t="n">
-        <v>0</v>
+        <v>-106339.167800643</v>
       </c>
       <c r="V34" t="n">
-        <v>0</v>
+        <v>-4586.264557766881</v>
       </c>
       <c r="W34" t="n">
-        <v>0</v>
+        <v>-5981.384428674952</v>
       </c>
       <c r="X34" t="n">
-        <v>0</v>
+        <v>-51454.93609388471</v>
       </c>
       <c r="Y34" t="n">
-        <v>0</v>
+        <v>-65196.39314599107</v>
       </c>
       <c r="Z34" t="n">
-        <v>0</v>
+        <v>-3184792.264178073</v>
       </c>
       <c r="AA34" t="n">
-        <v>0</v>
+        <v>-3212880.138917475</v>
       </c>
       <c r="AB34" t="n">
-        <v>0</v>
+        <v>0.5885452661649705</v>
       </c>
       <c r="AC34" t="n">
-        <v>0</v>
+        <v>0.3777823599213669</v>
       </c>
       <c r="AD34" t="n">
-        <v>0</v>
+        <v>0.03367237391366254</v>
       </c>
       <c r="AE34" t="n">
-        <v>0</v>
+        <v>0.5990367149221676</v>
       </c>
       <c r="AF34" t="n">
-        <v>0</v>
+        <v>0.3672685613655184</v>
       </c>
       <c r="AG34" t="n">
-        <v>0</v>
+        <v>0.03369472371231387</v>
       </c>
     </row>
     <row r="35">
@@ -4012,94 +4012,94 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>-33.32</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>0</v>
+        <v>21.42</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>19.9</v>
       </c>
       <c r="L35" t="n">
-        <v>0</v>
+        <v>-3859045.769862585</v>
       </c>
       <c r="M35" t="n">
-        <v>0</v>
+        <v>869976</v>
       </c>
       <c r="N35" t="n">
-        <v>0</v>
+        <v>1082880</v>
       </c>
       <c r="O35" t="n">
-        <v>0</v>
+        <v>156240</v>
       </c>
       <c r="P35" t="n">
-        <v>0</v>
+        <v>-369144</v>
       </c>
       <c r="Q35" t="n">
-        <v>0</v>
+        <v>-2989069.769862582</v>
       </c>
       <c r="R35" t="n">
-        <v>0</v>
+        <v>-90678.99879651524</v>
       </c>
       <c r="S35" t="n">
-        <v>0</v>
+        <v>-117422.6533466477</v>
       </c>
       <c r="T35" t="n">
-        <v>0</v>
+        <v>-75961.35973863814</v>
       </c>
       <c r="U35" t="n">
-        <v>0</v>
+        <v>-100767.5613856926</v>
       </c>
       <c r="V35" t="n">
-        <v>0</v>
+        <v>-4438.320539774383</v>
       </c>
       <c r="W35" t="n">
-        <v>0</v>
+        <v>-5788.436543878986</v>
       </c>
       <c r="X35" t="n">
-        <v>0</v>
+        <v>-48642.19494878705</v>
       </c>
       <c r="Y35" t="n">
-        <v>0</v>
+        <v>-61219.20551477723</v>
       </c>
       <c r="Z35" t="n">
-        <v>0</v>
+        <v>-3079748.768659097</v>
       </c>
       <c r="AA35" t="n">
-        <v>0</v>
+        <v>-3106492.423209229</v>
       </c>
       <c r="AB35" t="n">
-        <v>0</v>
+        <v>0.5886566636209803</v>
       </c>
       <c r="AC35" t="n">
-        <v>0</v>
+        <v>0.3769489157154948</v>
       </c>
       <c r="AD35" t="n">
-        <v>0</v>
+        <v>0.03439442066352481</v>
       </c>
       <c r="AE35" t="n">
-        <v>0</v>
+        <v>0.600610574846463</v>
       </c>
       <c r="AF35" t="n">
-        <v>0</v>
+        <v>0.3648882806158163</v>
       </c>
       <c r="AG35" t="n">
-        <v>0</v>
+        <v>0.03450114453772077</v>
       </c>
     </row>
     <row r="36">
@@ -4115,94 +4115,94 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>7.420000000000002</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>0.4200000000000017</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>-33.26</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>21.38</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>19.3</v>
       </c>
       <c r="L36" t="n">
-        <v>0</v>
+        <v>-3913548.468858003</v>
       </c>
       <c r="M36" t="n">
-        <v>0</v>
+        <v>824843.0399999991</v>
       </c>
       <c r="N36" t="n">
-        <v>0</v>
+        <v>1037850.239999999</v>
       </c>
       <c r="O36" t="n">
-        <v>0</v>
+        <v>161448</v>
       </c>
       <c r="P36" t="n">
-        <v>0</v>
+        <v>-374455.2</v>
       </c>
       <c r="Q36" t="n">
-        <v>0</v>
+        <v>-3088705.428858003</v>
       </c>
       <c r="R36" t="n">
-        <v>0</v>
+        <v>-88602.3075337909</v>
       </c>
       <c r="S36" t="n">
-        <v>0</v>
+        <v>-114246.2707100207</v>
       </c>
       <c r="T36" t="n">
-        <v>0</v>
+        <v>-72802.63319617177</v>
       </c>
       <c r="U36" t="n">
-        <v>0</v>
+        <v>-96577.31029140296</v>
       </c>
       <c r="V36" t="n">
-        <v>0</v>
+        <v>-4586.264557766881</v>
       </c>
       <c r="W36" t="n">
-        <v>0</v>
+        <v>-5981.384428674952</v>
       </c>
       <c r="X36" t="n">
-        <v>0</v>
+        <v>-49182.98801303355</v>
       </c>
       <c r="Y36" t="n">
-        <v>0</v>
+        <v>-61929.43806317863</v>
       </c>
       <c r="Z36" t="n">
-        <v>0</v>
+        <v>-3177307.736391794</v>
       </c>
       <c r="AA36" t="n">
-        <v>0</v>
+        <v>-3202951.699568024</v>
       </c>
       <c r="AB36" t="n">
-        <v>0</v>
+        <v>0.5751880265907278</v>
       </c>
       <c r="AC36" t="n">
-        <v>0</v>
+        <v>0.3885775084648965</v>
       </c>
       <c r="AD36" t="n">
-        <v>0</v>
+        <v>0.03623446494437571</v>
       </c>
       <c r="AE36" t="n">
-        <v>0</v>
+        <v>0.5871384680295532</v>
       </c>
       <c r="AF36" t="n">
-        <v>0</v>
+        <v>0.3764979090909986</v>
       </c>
       <c r="AG36" t="n">
-        <v>0</v>
+        <v>0.03636362287944827</v>
       </c>
     </row>
     <row r="37">
@@ -4218,94 +4218,94 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>5.990000000000002</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>-1.009999999999998</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>-33.61</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>0</v>
+        <v>20.98</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>18.62</v>
       </c>
       <c r="L37" t="n">
-        <v>0</v>
+        <v>-3724096.308858001</v>
       </c>
       <c r="M37" t="n">
-        <v>0</v>
+        <v>635390.8799999999</v>
       </c>
       <c r="N37" t="n">
-        <v>0</v>
+        <v>837833.2800000003</v>
       </c>
       <c r="O37" t="n">
-        <v>0</v>
+        <v>161448</v>
       </c>
       <c r="P37" t="n">
-        <v>0</v>
+        <v>-363890.4</v>
       </c>
       <c r="Q37" t="n">
-        <v>0</v>
+        <v>-3088705.428858003</v>
       </c>
       <c r="R37" t="n">
-        <v>0</v>
+        <v>-76695.93384311748</v>
       </c>
       <c r="S37" t="n">
-        <v>0</v>
+        <v>-97952.35535605573</v>
       </c>
       <c r="T37" t="n">
-        <v>0</v>
+        <v>-58771.93704111549</v>
       </c>
       <c r="U37" t="n">
-        <v>0</v>
+        <v>-77964.70197378864</v>
       </c>
       <c r="V37" t="n">
-        <v>0</v>
+        <v>-4586.264557766881</v>
       </c>
       <c r="W37" t="n">
-        <v>0</v>
+        <v>-5981.384428674952</v>
       </c>
       <c r="X37" t="n">
-        <v>0</v>
+        <v>-47676.37859138483</v>
       </c>
       <c r="Y37" t="n">
-        <v>0</v>
+        <v>-60087.19563523707</v>
       </c>
       <c r="Z37" t="n">
-        <v>0</v>
+        <v>-3165401.362701121</v>
       </c>
       <c r="AA37" t="n">
-        <v>0</v>
+        <v>-3186657.784214059</v>
       </c>
       <c r="AB37" t="n">
-        <v>0</v>
+        <v>0.5293120119912622</v>
       </c>
       <c r="AC37" t="n">
-        <v>0</v>
+        <v>0.4293831571181455</v>
       </c>
       <c r="AD37" t="n">
-        <v>0</v>
+        <v>0.04130483089059216</v>
       </c>
       <c r="AE37" t="n">
-        <v>0</v>
+        <v>0.541296434204571</v>
       </c>
       <c r="AF37" t="n">
-        <v>0</v>
+        <v>0.4171757720518323</v>
       </c>
       <c r="AG37" t="n">
-        <v>0</v>
+        <v>0.04152779374359689</v>
       </c>
     </row>
     <row r="38">
@@ -4321,94 +4321,94 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>4.870000000000005</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>-2.129999999999995</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>-34.23</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>0</v>
+        <v>19.9</v>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>19.2</v>
       </c>
       <c r="L38" t="n">
-        <v>0</v>
+        <v>-3453872.969862583</v>
       </c>
       <c r="M38" t="n">
-        <v>0</v>
+        <v>464803.2000000002</v>
       </c>
       <c r="N38" t="n">
-        <v>0</v>
+        <v>659203.2000000002</v>
       </c>
       <c r="O38" t="n">
-        <v>0</v>
+        <v>156240</v>
       </c>
       <c r="P38" t="n">
-        <v>0</v>
+        <v>-350640</v>
       </c>
       <c r="Q38" t="n">
-        <v>0</v>
+        <v>-2989069.769862582</v>
       </c>
       <c r="R38" t="n">
-        <v>0</v>
+        <v>-66662.5203837812</v>
       </c>
       <c r="S38" t="n">
-        <v>0</v>
+        <v>-84186.67004258973</v>
       </c>
       <c r="T38" t="n">
-        <v>0</v>
+        <v>-46241.47774089546</v>
       </c>
       <c r="U38" t="n">
-        <v>0</v>
+        <v>-61342.25299353994</v>
       </c>
       <c r="V38" t="n">
-        <v>0</v>
+        <v>-4438.320539774383</v>
       </c>
       <c r="W38" t="n">
-        <v>0</v>
+        <v>-5788.436543878986</v>
       </c>
       <c r="X38" t="n">
-        <v>0</v>
+        <v>-46114.3397081189</v>
       </c>
       <c r="Y38" t="n">
-        <v>0</v>
+        <v>-58373.59468950734</v>
       </c>
       <c r="Z38" t="n">
-        <v>0</v>
+        <v>-3055732.290246363</v>
       </c>
       <c r="AA38" t="n">
-        <v>0</v>
+        <v>-3073256.439905172</v>
       </c>
       <c r="AB38" t="n">
-        <v>0</v>
+        <v>0.4777301466980513</v>
       </c>
       <c r="AC38" t="n">
-        <v>0</v>
+        <v>0.4764166577263194</v>
       </c>
       <c r="AD38" t="n">
-        <v>0</v>
+        <v>0.04585319557562934</v>
       </c>
       <c r="AE38" t="n">
-        <v>0</v>
+        <v>0.4887662072366076</v>
       </c>
       <c r="AF38" t="n">
-        <v>0</v>
+        <v>0.4651123668731589</v>
       </c>
       <c r="AG38" t="n">
-        <v>0</v>
+        <v>0.04612142589023355</v>
       </c>
     </row>
     <row r="39">
@@ -4424,94 +4424,94 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>-34.54</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>0</v>
+        <v>19.14</v>
       </c>
       <c r="K39" t="n">
-        <v>0</v>
+        <v>20.4</v>
       </c>
       <c r="L39" t="n">
-        <v>0</v>
+        <v>-3579447.828858003</v>
       </c>
       <c r="M39" t="n">
-        <v>0</v>
+        <v>490742.4000000004</v>
       </c>
       <c r="N39" t="n">
-        <v>0</v>
+        <v>699359.9999999991</v>
       </c>
       <c r="O39" t="n">
-        <v>0</v>
+        <v>161448</v>
       </c>
       <c r="P39" t="n">
-        <v>0</v>
+        <v>-370065.6</v>
       </c>
       <c r="Q39" t="n">
-        <v>0</v>
+        <v>-3088705.428858003</v>
       </c>
       <c r="R39" t="n">
-        <v>0</v>
+        <v>-70903.94102408546</v>
       </c>
       <c r="S39" t="n">
-        <v>0</v>
+        <v>-89598.82184417429</v>
       </c>
       <c r="T39" t="n">
-        <v>0</v>
+        <v>-49058.37816453623</v>
       </c>
       <c r="U39" t="n">
-        <v>0</v>
+        <v>-65079.05006159223</v>
       </c>
       <c r="V39" t="n">
-        <v>0</v>
+        <v>-4586.264557766881</v>
       </c>
       <c r="W39" t="n">
-        <v>0</v>
+        <v>-5981.384428674952</v>
       </c>
       <c r="X39" t="n">
-        <v>0</v>
+        <v>-49155.8612530796</v>
       </c>
       <c r="Y39" t="n">
-        <v>0</v>
+        <v>-62307.32114934881</v>
       </c>
       <c r="Z39" t="n">
-        <v>0</v>
+        <v>-3159609.369882089</v>
       </c>
       <c r="AA39" t="n">
-        <v>0</v>
+        <v>-3178304.250702177</v>
       </c>
       <c r="AB39" t="n">
-        <v>0</v>
+        <v>0.4772192379162272</v>
       </c>
       <c r="AC39" t="n">
-        <v>0</v>
+        <v>0.4781675123387604</v>
       </c>
       <c r="AD39" t="n">
-        <v>0</v>
+        <v>0.04461324974501232</v>
       </c>
       <c r="AE39" t="n">
-        <v>0</v>
+        <v>0.4879668983667064</v>
       </c>
       <c r="AF39" t="n">
-        <v>0</v>
+        <v>0.4671842969129252</v>
       </c>
       <c r="AG39" t="n">
-        <v>0</v>
+        <v>0.04484880472036842</v>
       </c>
     </row>
     <row r="40">
@@ -4527,94 +4527,94 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>6.519999999999996</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>-0.480000000000004</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>-34.5</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>0</v>
+        <v>19.22</v>
       </c>
       <c r="K40" t="n">
-        <v>0</v>
+        <v>21.8</v>
       </c>
       <c r="L40" t="n">
-        <v>0</v>
+        <v>-3654032.969862584</v>
       </c>
       <c r="M40" t="n">
-        <v>0</v>
+        <v>664963.2000000002</v>
       </c>
       <c r="N40" t="n">
-        <v>0</v>
+        <v>882547.2000000002</v>
       </c>
       <c r="O40" t="n">
-        <v>0</v>
+        <v>156240</v>
       </c>
       <c r="P40" t="n">
-        <v>0</v>
+        <v>-373824</v>
       </c>
       <c r="Q40" t="n">
-        <v>0</v>
+        <v>-2989069.769862582</v>
       </c>
       <c r="R40" t="n">
-        <v>0</v>
+        <v>-81203.75846946613</v>
       </c>
       <c r="S40" t="n">
-        <v>0</v>
+        <v>-103230.2747930372</v>
       </c>
       <c r="T40" t="n">
-        <v>0</v>
+        <v>-61908.50818699083</v>
       </c>
       <c r="U40" t="n">
-        <v>0</v>
+        <v>-82125.56252934023</v>
       </c>
       <c r="V40" t="n">
-        <v>0</v>
+        <v>-4438.320539774383</v>
       </c>
       <c r="W40" t="n">
-        <v>0</v>
+        <v>-5788.436543878986</v>
       </c>
       <c r="X40" t="n">
-        <v>0</v>
+        <v>-50081.83455280834</v>
       </c>
       <c r="Y40" t="n">
-        <v>0</v>
+        <v>-63432.71077665011</v>
       </c>
       <c r="Z40" t="n">
-        <v>0</v>
+        <v>-3070273.528332048</v>
       </c>
       <c r="AA40" t="n">
-        <v>0</v>
+        <v>-3092300.044655619</v>
       </c>
       <c r="AB40" t="n">
-        <v>0</v>
+        <v>0.5317290986870942</v>
       </c>
       <c r="AC40" t="n">
-        <v>0</v>
+        <v>0.4301503868729444</v>
       </c>
       <c r="AD40" t="n">
-        <v>0</v>
+        <v>0.03812051443996136</v>
       </c>
       <c r="AE40" t="n">
-        <v>0</v>
+        <v>0.5426319647834165</v>
       </c>
       <c r="AF40" t="n">
-        <v>0</v>
+        <v>0.4191218351530281</v>
       </c>
       <c r="AG40" t="n">
-        <v>0</v>
+        <v>0.0382462000635555</v>
       </c>
     </row>
     <row r="41">
@@ -4630,94 +4630,94 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>744</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>6.149999999999999</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>-0.8500000000000014</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>-34.71</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>19.26</v>
       </c>
       <c r="K41" t="n">
-        <v>0</v>
+        <v>21.6</v>
       </c>
       <c r="L41" t="n">
-        <v>0</v>
+        <v>-3726015.828858003</v>
       </c>
       <c r="M41" t="n">
-        <v>0</v>
+        <v>637310.3999999994</v>
       </c>
       <c r="N41" t="n">
-        <v>0</v>
+        <v>860212.7999999998</v>
       </c>
       <c r="O41" t="n">
-        <v>0</v>
+        <v>161448</v>
       </c>
       <c r="P41" t="n">
-        <v>0</v>
+        <v>-384350.4</v>
       </c>
       <c r="Q41" t="n">
-        <v>0</v>
+        <v>-3088705.428858003</v>
       </c>
       <c r="R41" t="n">
-        <v>0</v>
+        <v>-80748.88635470255</v>
       </c>
       <c r="S41" t="n">
-        <v>0</v>
+        <v>-102654.8534772083</v>
       </c>
       <c r="T41" t="n">
-        <v>0</v>
+        <v>-60341.80514238076</v>
       </c>
       <c r="U41" t="n">
-        <v>0</v>
+        <v>-80047.23157575965</v>
       </c>
       <c r="V41" t="n">
-        <v>0</v>
+        <v>-4586.264557766881</v>
       </c>
       <c r="W41" t="n">
-        <v>0</v>
+        <v>-5981.384428674952</v>
       </c>
       <c r="X41" t="n">
-        <v>0</v>
+        <v>-51409.08759000062</v>
       </c>
       <c r="Y41" t="n">
-        <v>0</v>
+        <v>-65123.16870846189</v>
       </c>
       <c r="Z41" t="n">
-        <v>0</v>
+        <v>-3169454.315212706</v>
       </c>
       <c r="AA41" t="n">
-        <v>0</v>
+        <v>-3191360.282335212</v>
       </c>
       <c r="AB41" t="n">
-        <v>0</v>
+        <v>0.518680416024663</v>
       </c>
       <c r="AC41" t="n">
-        <v>0</v>
+        <v>0.4418974022356835</v>
       </c>
       <c r="AD41" t="n">
-        <v>0</v>
+        <v>0.03942218173965351</v>
       </c>
       <c r="AE41" t="n">
-        <v>0</v>
+        <v>0.5295817824963458</v>
       </c>
       <c r="AF41" t="n">
-        <v>0</v>
+        <v>0.4308461777818855</v>
       </c>
       <c r="AG41" t="n">
-        <v>0</v>
+        <v>0.03957203972176857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>